<commit_message>
Incluindo mais cenários de testes do login
</commit_message>
<xml_diff>
--- a/docs/plano_testes.xlsx
+++ b/docs/plano_testes.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Diversos\Meus cursos\Qualiters club\Desafios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81CD61A-F531-4DCC-9DEB-5395EB003C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218CB5FB-2CBA-4AE1-A321-9FD01419C871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14970" windowHeight="15585" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="macros" sheetId="2" r:id="rId1"/>
     <sheet name="Suite - Tela Inicial" sheetId="5" r:id="rId2"/>
     <sheet name="Suite - My Account" sheetId="8" r:id="rId3"/>
-    <sheet name="Suite - MyAccount LostPassword" sheetId="10" r:id="rId4"/>
+    <sheet name="Suite - MyAccount-LostPassword" sheetId="10" r:id="rId4"/>
     <sheet name="Suite - Login" sheetId="9" r:id="rId5"/>
+    <sheet name="Suite - Go Shop" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="148">
   <si>
     <t>Tipos de Teste</t>
   </si>
@@ -194,9 +195,6 @@
 QUANDO acessar o menu superior "My Account"</t>
   </si>
   <si>
-    <t>Exibir menu superior "My Account" com opções "Login" e "Register" na "tela inicial"</t>
-  </si>
-  <si>
     <t>Validar tela inicial</t>
   </si>
   <si>
@@ -213,23 +211,10 @@
     <t>ENTÃO deve exibir os seguintes menus "Shop", "My Account", "Test Cases", "AT Suite", "Demo Site" e "Items"</t>
   </si>
   <si>
-    <t>DADO que estou no menu superior "My Account"
-QUANDO preencher os campos "Email address" e "Password" com dados válidos</t>
-  </si>
-  <si>
-    <t>ENTÃO deve ser direcionado para tela de login "Hello..."</t>
-  </si>
-  <si>
     <t>Acessar menu superior "My Account"</t>
   </si>
   <si>
     <t>Exibir menu superior "My Account" com opções "Login" e "Register"</t>
-  </si>
-  <si>
-    <t>ENTÃO deve retornar a seguinte mensagem: "Error: Please enter an account password."</t>
-  </si>
-  <si>
-    <t>ENTÃO sistema não deverá registrar</t>
   </si>
   <si>
     <t>https://practice.automationtesting.in/my-account/</t>
@@ -238,28 +223,11 @@
     <t>Dados válidos e inválidos</t>
   </si>
   <si>
-    <t>ENTÃO deve exibir a seguinte mensagem: "Error: Please provide a valid email address."</t>
-  </si>
-  <si>
-    <t>ENTÃO deve exibir a seguinte mensagem: "Error: Please provide a valid email address"</t>
-  </si>
-  <si>
-    <t>Validar o Login</t>
-  </si>
-  <si>
     <t>Acessar menu superior "My Account - Login"</t>
-  </si>
-  <si>
-    <t>Dados válidos</t>
   </si>
   <si>
     <t>DADO que estou no menu superior "My Account"
 QUANDO preencher os campos "Email address" e "Password" com dados válidos
-E acionar botão "REGISTER"</t>
-  </si>
-  <si>
-    <t>DADO que estou no menu superior "My Account"
-QUANDO acionar o botão "Register" sem preencher os campos
 E acionar botão "REGISTER"</t>
   </si>
   <si>
@@ -269,51 +237,13 @@
   </si>
   <si>
     <t>DADO que estou no menu superior "My Account"
-QUANDO preencher o campo "Email address" com dado inválido
+QUANDO não preencher o campo "Password"
 E acionar botão "REGISTER"</t>
   </si>
   <si>
     <t>DADO que estou no menu superior "My Account"
 QUANDO não preencher o campo "Password"
-E acionar botão "REGISTER"</t>
-  </si>
-  <si>
-    <t>DADO que estou no menu superior "My Account"
-QUANDO preencher os campos "Email address" e "Password" com dados válidos
 E acionar botão "LOGIN"</t>
-  </si>
-  <si>
-    <t>DADO que estou no menu superior "My Account"
-QUANDO acionar o botão "Register" sem preencher os campos
-E acionar botão "LOGIN"</t>
-  </si>
-  <si>
-    <t>DADO que estou no menu superior "My Account"
-QUANDO não preencher o campo "Email address"
-E acionar botão "LOGIN"</t>
-  </si>
-  <si>
-    <t>DADO que estou no menu superior "My Account"
-QUANDO preencher o campo "Email address" com dado inválido
-E acionar botão "LOGIN"</t>
-  </si>
-  <si>
-    <t>DADO que estou no menu superior "My Account"
-QUANDO não preencher o campo "Password"
-E acionar botão "LOGIN"</t>
-  </si>
-  <si>
-    <t>DADO que estou no menu superior "My Account"
-QUANDO preencher os campos "Email address" e "Password" com dados válidos
-E marcar opção "Remenber me"
-E acionar botão "LOGIN"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENTÃO sistema deve guardar os dados de login
-</t>
-  </si>
-  <si>
-    <t>ENTÃO deve ser direcionado para tela "Lost your password? Please enter your username or email address. You will receive a link to create a new password via email."</t>
   </si>
   <si>
     <t>DADO que estou no menu superior "My Account"
@@ -401,6 +331,242 @@
   </si>
   <si>
     <t>ENTÃO deve exibir a mensagem: "Error: Invalid username or email."</t>
+  </si>
+  <si>
+    <t>ENTÃO deve ser direcionado para a tela de Lost your password? com a mensagem: "Lost your password? Please enter your username or email address. You will receive a link to create a new password via email."</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir o campo "Username or email"
+E o botão "RESET PASSWORD"</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"
+QUANDO preencher o campo "Username or email" com nome de usuário válido cadastrado
+E acionar o botão "RESET PASSWORD"</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"
+QUANDO preencher o campo "Username or email" com e-mail válido cadastrado
+E acionar o botão "RESET PASSWORD"</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"
+QUANDO deixar o campo "Username or email" em branco
+E acionar o botão "RESET PASSWORD"</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"
+QUANDO preencher o campo "Username or email" com um e-mail não cadastrado
+E acionar o botão "RESET PASSWORD"</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"
+QUANDO preencher o campo "Username or email" com formato inválido (ex: "user@")
+E acionar o botão "RESET PASSWORD"</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir uma mensagem informando que o e-mail é inválido</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"
+QUANDO preencher o campo "Username or email" com caracteres especiais ou código malicioso (ex: "&lt;script&gt;")
+E acionar o botão "RESET PASSWORD"</t>
+  </si>
+  <si>
+    <t>ENTÃO o sistema deve impedir o envio e exibir uma mensagem de erro genérica
+E não deve executar o código inserido (proteção contra XSS)</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"
+QUANDO preencher o campo "Username or email" corretamente
+E houver falha temporária no servidor de e-mail</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"
+QUANDO o usuário acionar o botão "RESET PASSWORD"
+E a conexão com a internet for perdida antes da requisição ser concluída</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem "Connection error. Please check your internet and try again."</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"
+QUANDO o link de redefinição enviado por e-mail for acessado após o prazo de validade</t>
+  </si>
+  <si>
+    <t>DADO que estou na tela "Lost your password"
+QUANDO o link de redefinição enviado for utilizado mais de uma vez</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem "This password reset link has already been used. Please request a new one."</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem: "This password reset link has expired. Please request a new one."</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem: "Connection error. Please check your internet and try again."</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem: "An error occurred while sending the email. Please try again later."</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem: "Invalid username or email."</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem: "Please enter your username or email address."</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem: "Password reset email has been sent"
+E o sistema deve enviar o link de redefinição de senha para o e-mail associado ao usuário</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem: "Password reset email has been sent"
+E o sistema deve enviar o link de redefinição de senha para o e-mail informado</t>
+  </si>
+  <si>
+    <t>Botão "Lost your password?"</t>
+  </si>
+  <si>
+    <t>Validar tela "Lost your password?"</t>
+  </si>
+  <si>
+    <t>testes#123586</t>
+  </si>
+  <si>
+    <t>Validar tela de Login</t>
+  </si>
+  <si>
+    <t>DADO que estou logada com sucesso na área "My Account"</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem de boas-vindas com o nome do usuário
+E o menu com as opções "Dashboard", "Orders", "Downloads", "Addresses", "Account Details" e "Logout"</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO acessar a opção "Dashboard"</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir o resumo da conta do usuário e as informações principais do perfil</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO acessar a opção "Orders"</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO acessar a opção "Downloads"</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO acessar a opção "Addresses"</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO acessar a opção "Account Details"</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO alterar informações válidas no "Account Details"
+E acionar o botão "Save changes"</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO clicar em "Logout"</t>
+  </si>
+  <si>
+    <t>ENTÃO deve encerrar a sessão atual
+E redirecionar para a tela de login</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO tentar alterar o "Email address" para um formato inválido (ex: "user@")
+E acionar o botão "Save changes"</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem "Please enter a valid email address."</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO deixar os campos obrigatórios (ex: "First name") em branco
+E acionar o botão "Save changes"</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem "First name is a required field."</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO tentar alterar a senha atual informando uma senha incorreta</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem "Current password is incorrect."</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO tentar alterar a senha nova para uma igual à atual</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem "New password cannot be the same as the current password."</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO tentar salvar informações com campos contendo caracteres especiais ou código malicioso</t>
+  </si>
+  <si>
+    <t>ENTÃO o sistema deve impedir o envio
+E exibir uma mensagem de erro genérica (proteção contra XSS)</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO a sessão expirar após um tempo de inatividade</t>
+  </si>
+  <si>
+    <t>ENTÃO deve redirecionar automaticamente para a tela de login
+E exibir a mensagem "Your session has expired. Please log in again."</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO houver falha temporária no servidor ao salvar alterações do perfil</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem "An error occurred while saving your changes. Please try again later."</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO perder a conexão com a internet durante a atualização dos dados</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO tentar acessar uma seção restrita sem permissão</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a mensagem "You do not have permission to access this section."</t>
+  </si>
+  <si>
+    <t>DADO que estou logada na área "My Account"
+QUANDO ocorrer falha de sincronização entre o cliente e o servidor</t>
+  </si>
+  <si>
+    <t>ENTÃO o sistema deve exibir uma mensagem "Your data could not be updated. Please refresh and try again."</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a lista de pedidos caso o usuário tenha</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir a lista de produtos disponíveis para download caso usuário tenha</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir os endereços de cobrança e entrega caso usuário tenha cadastrado</t>
+  </si>
+  <si>
+    <t>ENTÃO deve exibir os campos "First name", "Last name", "Password change" E o botão "SAVE CHANGES"</t>
+  </si>
+  <si>
+    <t>ENTÃO deve salvar as alterações 
+E deve exibir a mensagem: "Account details changed successfully."</t>
   </si>
 </sst>
 </file>
@@ -496,7 +662,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,6 +691,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -609,7 +781,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -674,6 +846,9 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -702,8 +877,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -964,12 +1139,12 @@
         <v>5</v>
       </c>
       <c r="G1" s="3"/>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1007,10 +1182,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1048,10 +1223,10 @@
         <v>17</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1089,10 +1264,10 @@
         <v>22</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1126,10 +1301,10 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -30028,7 +30203,7 @@
   <dimension ref="A1:W994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -30046,83 +30221,83 @@
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>50</v>
+      <c r="B3" s="31" t="s">
+        <v>49</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>51</v>
+      <c r="D5" s="27" t="s">
+        <v>50</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>52</v>
+      <c r="B6" s="27" t="s">
+        <v>51</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:23" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
@@ -30190,8 +30365,12 @@
       <c r="B10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="E10" s="19" t="s">
         <v>44</v>
       </c>
@@ -30205,12 +30384,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>53</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="19" t="s">
-        <v>54</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="16"/>
@@ -30224,8 +30407,12 @@
       <c r="B12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="C12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="E12" s="19" t="s">
         <v>47</v>
       </c>
@@ -34232,10 +34419,10 @@
   <sheetPr codeName="Planilha3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W993"/>
+  <dimension ref="A1:W992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -34253,83 +34440,83 @@
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>61</v>
+      <c r="B4" s="32" t="s">
+        <v>56</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:23" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>62</v>
+      <c r="D5" s="27" t="s">
+        <v>57</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>58</v>
+      <c r="B6" s="27" t="s">
+        <v>55</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:23" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
@@ -34390,238 +34577,278 @@
       <c r="V9" s="18"/>
       <c r="W9" s="18"/>
     </row>
-    <row r="10" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
+    <row r="10" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="24">
         <v>1</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="D10" s="16"/>
-      <c r="E10" s="19" t="s">
-        <v>47</v>
+      <c r="E10" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="16"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
+    <row r="11" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="24">
         <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="D11" s="16"/>
-      <c r="E11" s="19" t="s">
-        <v>83</v>
+      <c r="E11" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="16"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:23" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
+    <row r="12" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="24">
         <v>3</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="D12" s="16"/>
-      <c r="E12" s="19" t="s">
-        <v>85</v>
+      <c r="E12" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="16"/>
       <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="16">
+      <c r="A13" s="24">
         <v>4</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="19" t="s">
-        <v>85</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="16"/>
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="16">
+      <c r="A14" s="24">
         <v>5</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="D14" s="16"/>
-      <c r="E14" s="19" t="s">
-        <v>88</v>
+      <c r="E14" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="16"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="16">
+    <row r="15" spans="1:23" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="24">
         <v>6</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="19" t="s">
-        <v>87</v>
+      <c r="C15" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="16"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:23" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="16">
+    <row r="16" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="24">
         <v>7</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>83</v>
+      <c r="C16" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="16"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="16">
+    <row r="17" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="24">
         <v>8</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
-      <c r="C17" s="16"/>
+      <c r="C17" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="D17" s="16"/>
-      <c r="E17" s="19" t="s">
-        <v>85</v>
+      <c r="E17" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="16"/>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="16">
+      <c r="A18" s="24">
         <v>9</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="D18" s="16"/>
-      <c r="E18" s="19" t="s">
-        <v>85</v>
+      <c r="E18" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="16"/>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="16">
+      <c r="A19" s="24">
         <v>10</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="19" t="s">
-        <v>85</v>
+      <c r="E19" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="16"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="16">
+    <row r="20" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="24">
         <v>11</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="19" t="s">
-        <v>87</v>
+      <c r="E20" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="16"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="16">
+    <row r="21" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="24">
         <v>12</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="19" t="s">
-        <v>94</v>
+      <c r="E21" s="10" t="s">
+        <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="16">
+      <c r="F21" s="17"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="24">
         <v>13</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="19" t="s">
-        <v>96</v>
+      <c r="E22" s="10" t="s">
+        <v>80</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="16">
+      <c r="F22" s="17"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="24">
         <v>14</v>
       </c>
-      <c r="B23" s="34" t="s">
-        <v>97</v>
+      <c r="B23" s="10" t="s">
+        <v>81</v>
       </c>
-      <c r="E23" s="19" t="s">
-        <v>98</v>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="10" t="s">
+        <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="16">
+      <c r="F23" s="17"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="24">
         <v>15</v>
       </c>
-      <c r="B24" s="34" t="s">
-        <v>99</v>
+      <c r="B24" s="10" t="s">
+        <v>83</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>100</v>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="10" t="s">
+        <v>84</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="16">
+      <c r="F24" s="17"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="24">
         <v>16</v>
       </c>
-      <c r="B25" s="34" t="s">
-        <v>101</v>
+      <c r="B25" s="10" t="s">
+        <v>63</v>
       </c>
-      <c r="E25" s="19" t="s">
-        <v>102</v>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="10" t="s">
+        <v>85</v>
       </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B26" s="11"/>
@@ -38490,10 +38717,6 @@
     <row r="992" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B992" s="11"/>
       <c r="E992" s="20"/>
-    </row>
-    <row r="993" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B993" s="11"/>
-      <c r="E993" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -38523,12 +38746,6 @@
           </x14:formula1>
           <xm:sqref>B1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{F28A902C-C7AD-4C8D-AF3C-80432EB981B4}">
-          <x14:formula1>
-            <xm:f>macros!$F$2:$F$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>H10:H20</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{E4B3B12D-116E-48AC-B0E4-3542BA0C0784}">
           <x14:formula1>
             <xm:f>macros!$D$2:$D$5</xm:f>
@@ -38539,13 +38756,19 @@
           <x14:formula1>
             <xm:f>macros!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C10:C15 C17:C20</xm:sqref>
+          <xm:sqref>C10:C25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{4BD05CD4-C2E9-4BC8-B363-813601B0C05B}">
           <x14:formula1>
             <xm:f>macros!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D10:D15 D17:D20</xm:sqref>
+          <xm:sqref>D16:D25 D10:D14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{F28A902C-C7AD-4C8D-AF3C-80432EB981B4}">
+          <x14:formula1>
+            <xm:f>macros!$F$2:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>H10:H25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -38561,7 +38784,7 @@
   <dimension ref="A1:W993"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -38579,83 +38802,83 @@
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>43</v>
+      <c r="B3" s="31" t="s">
+        <v>110</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>82</v>
+      <c r="B4" s="32" t="s">
+        <v>64</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:23" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>62</v>
+      <c r="D5" s="27" t="s">
+        <v>57</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>58</v>
+      <c r="B6" s="27" t="s">
+        <v>109</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:23" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
@@ -38721,12 +38944,12 @@
         <v>1</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="19" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="16"/>
@@ -38737,28 +38960,28 @@
         <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="19" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="16"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <v>3</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="19" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="16"/>
@@ -38769,12 +38992,12 @@
         <v>4</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="19" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="16"/>
@@ -38785,74 +39008,74 @@
         <v>5</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="19" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="16"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A15" s="16">
         <v>6</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="19" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="16"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A16" s="16">
         <v>7</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="16"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A17" s="16">
         <v>8</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="19" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="16"/>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A18" s="16">
         <v>9</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="19" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="16"/>
@@ -38863,55 +39086,35 @@
         <v>10</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="19" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="16"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="16">
         <v>11</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="19" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="16"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="16">
-        <v>12</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="16">
-        <v>13</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
+    <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B23" s="11"/>
       <c r="E23" s="20"/>
@@ -42798,12 +43001,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B6:G6"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="B6" xr:uid="{0FF2EACA-BB39-4535-A585-52B4E43A9586}">
@@ -42822,13 +43025,13 @@
           <x14:formula1>
             <xm:f>macros!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D10:D15 D17:D20</xm:sqref>
+          <xm:sqref>D10:D15 D17:D19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{45753ED9-7F59-4CDE-A748-06B90B1367E5}">
           <x14:formula1>
             <xm:f>macros!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C10:C15 C17:C20</xm:sqref>
+          <xm:sqref>C10:C15 D20 C17:C20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{D9A3FFF8-517C-49A5-B3EE-90C0443DB0A9}">
           <x14:formula1>
@@ -42861,8 +43064,8 @@
   </sheetPr>
   <dimension ref="A1:W994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -42880,83 +43083,84 @@
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>65</v>
+      <c r="B3" s="31" t="s">
+        <v>112</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>42</v>
+      <c r="B4" s="32" t="s">
+        <v>56</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:23" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>67</v>
+      <c r="D5" s="27" t="s">
+        <v>57</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-    </row>
-    <row r="6" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
+      <c r="I5" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:23" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
@@ -43017,120 +43221,328 @@
       <c r="V9" s="18"/>
       <c r="W9" s="18"/>
     </row>
-    <row r="10" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>1</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="19" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="16"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
-        <f t="shared" ref="A11" si="0">A10+1</f>
+        <f t="shared" ref="A11:A27" si="0">A10+1</f>
         <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="19" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="16"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="11"/>
-      <c r="E12" s="20"/>
-    </row>
-    <row r="13" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="11"/>
-      <c r="E13" s="20"/>
-    </row>
-    <row r="14" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="11"/>
-      <c r="E14" s="20"/>
-    </row>
-    <row r="15" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="11"/>
-      <c r="E15" s="20"/>
-    </row>
-    <row r="16" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B16" s="11"/>
-      <c r="E16" s="20"/>
-    </row>
-    <row r="17" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B17" s="11"/>
-      <c r="E17" s="20"/>
-    </row>
-    <row r="18" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="11"/>
-      <c r="E18" s="20"/>
-    </row>
-    <row r="19" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B19" s="11"/>
-      <c r="E19" s="20"/>
-    </row>
-    <row r="20" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B20" s="11"/>
-      <c r="E20" s="20"/>
-    </row>
-    <row r="21" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B21" s="11"/>
-      <c r="E21" s="20"/>
-    </row>
-    <row r="22" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B22" s="11"/>
-      <c r="E22" s="20"/>
-    </row>
-    <row r="23" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B23" s="11"/>
-      <c r="E23" s="20"/>
-    </row>
-    <row r="24" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B24" s="11"/>
-      <c r="E24" s="20"/>
-    </row>
-    <row r="25" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B25" s="11"/>
-      <c r="E25" s="20"/>
-    </row>
-    <row r="26" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B26" s="11"/>
-      <c r="E26" s="20"/>
-    </row>
-    <row r="27" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B27" s="11"/>
-      <c r="E27" s="20"/>
-    </row>
-    <row r="28" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="16">
+        <f>A17+1</f>
+        <v>8</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="35">
+        <f>A15+1</f>
+        <v>7</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="16">
+        <f>A16+1</f>
+        <v>9</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="16">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="12"/>
+    </row>
+    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="16">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="12"/>
+    </row>
+    <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B28" s="11"/>
       <c r="E28" s="20"/>
     </row>
-    <row r="29" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B29" s="11"/>
       <c r="E29" s="20"/>
     </row>
-    <row r="30" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B30" s="11"/>
       <c r="E30" s="20"/>
     </row>
-    <row r="31" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B31" s="11"/>
       <c r="E31" s="20"/>
     </row>
-    <row r="32" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B32" s="11"/>
       <c r="E32" s="20"/>
     </row>
@@ -47004,29 +47416,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{E98861B1-B873-4597-BC8C-2B577B4356CE}">
-          <x14:formula1>
-            <xm:f>macros!$B$2:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>D10:D11</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{984DFAA4-DA1B-4273-8667-742082635EED}">
-          <x14:formula1>
-            <xm:f>macros!$C$2:$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C10:C11</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{63070E1A-DA05-4FDF-8A34-2550E0D0D7F1}">
           <x14:formula1>
             <xm:f>macros!$D$2:$D$5</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{FFFE94E2-B9BE-4313-B5E9-E9501D0F00C7}">
-          <x14:formula1>
-            <xm:f>macros!$F$2:$F$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>H10:H11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{5880063E-6DA5-4D17-BB66-3EF995B7C37A}">
           <x14:formula1>
@@ -47034,8 +47428,40 @@
           </x14:formula1>
           <xm:sqref>B1</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{E98861B1-B873-4597-BC8C-2B577B4356CE}">
+          <x14:formula1>
+            <xm:f>macros!$B$2:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>D18:D27 D10:D17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{984DFAA4-DA1B-4273-8667-742082635EED}">
+          <x14:formula1>
+            <xm:f>macros!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C18:C27 C10:C17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{FFFE94E2-B9BE-4313-B5E9-E9501D0F00C7}">
+          <x14:formula1>
+            <xm:f>macros!$F$2:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>H18:H27 H10:H17</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CCEF96-439C-4F92-B4DA-21EAD960EC02}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Alterando padrão de escrita gherkin
</commit_message>
<xml_diff>
--- a/docs/plano_testes.xlsx
+++ b/docs/plano_testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Diversos\Meus cursos\Qualiters club\Desafios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218CB5FB-2CBA-4AE1-A321-9FD01419C871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A131B68C-5A56-4755-9A80-1ACC784A0AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,9 +390,6 @@
 E a conexão com a internet for perdida antes da requisição ser concluída</t>
   </si>
   <si>
-    <t>ENTÃO deve exibir a mensagem "Connection error. Please check your internet and try again."</t>
-  </si>
-  <si>
     <t>DADO que estou na tela "Lost your password"
 QUANDO o link de redefinição enviado por e-mail for acessado após o prazo de validade</t>
   </si>
@@ -439,134 +436,138 @@
     <t>Validar tela de Login</t>
   </si>
   <si>
-    <t>DADO que estou logada com sucesso na área "My Account"</t>
+    <t>ENTÃO deve ser exibida a mensagem "Please enter a valid email address."</t>
   </si>
   <si>
-    <t>ENTÃO deve exibir a mensagem de boas-vindas com o nome do usuário
+    <t xml:space="preserve">DADO que estou autenticada com sucesso na área "My Account"  </t>
+  </si>
+  <si>
+    <t>ENTÃO deve ser exibida a mensagem de boas-vindas com o nome do usuário  
 E o menu com as opções "Dashboard", "Orders", "Downloads", "Addresses", "Account Details" e "Logout"</t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO acessar a opção "Dashboard"</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO acesso a opção "Dashboard"  </t>
   </si>
   <si>
-    <t>ENTÃO deve exibir o resumo da conta do usuário e as informações principais do perfil</t>
+    <t>ENTÃO deve ser exibido o resumo da conta e as informações principais do perfil</t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO acessar a opção "Orders"</t>
+    <t>DADO que estou autenticada na área "My Account"  
+QUANDO acesso a opção "Orders"</t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO acessar a opção "Downloads"</t>
+    <t>ENTÃO deve ser exibida a lista de pedidos, caso o usuário possua</t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO acessar a opção "Addresses"</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO acesso a opção "Downloads"  </t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO acessar a opção "Account Details"</t>
+    <t>ENTÃO deve ser exibida a lista de produtos disponíveis para download, caso o usuário possua</t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO alterar informações válidas no "Account Details"
-E acionar o botão "Save changes"</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO acesso a opção "Addresses" </t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO clicar em "Logout"</t>
+    <t>ENTÃO devem ser exibidos os endereços de cobrança e entrega, caso o usuário tenha cadastrado</t>
   </si>
   <si>
-    <t>ENTÃO deve encerrar a sessão atual
-E redirecionar para a tela de login</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO acesso a opção "Account Details"  </t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO tentar alterar o "Email address" para um formato inválido (ex: "user@")
-E acionar o botão "Save changes"</t>
+    <t>ENTÃO devem ser exibidos os campos "First name", "Last name", "Password change" e o botão "Save changes"</t>
   </si>
   <si>
-    <t>ENTÃO deve exibir a mensagem "Please enter a valid email address."</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO altero informações válidas na seção "Account Details"  
+E clico no botão "Save changes"  </t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO deixar os campos obrigatórios (ex: "First name") em branco
-E acionar o botão "Save changes"</t>
+    <t>ENTÃO as alterações devem ser salvas  
+E deve ser exibida a mensagem "Account details changed successfully."</t>
   </si>
   <si>
-    <t>ENTÃO deve exibir a mensagem "First name is a required field."</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO clico em "Logout"  </t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO tentar alterar a senha atual informando uma senha incorreta</t>
+    <t>ENTÃO a sessão atual deve ser encerrada  
+E o sistema deve redirecionar para a tela de login</t>
   </si>
   <si>
-    <t>ENTÃO deve exibir a mensagem "Current password is incorrect."</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+E acesso a seção "Account Details"  
+QUANDO altero o campo "Email address" para um formato inválido (ex: "user@")  
+E clico no botão "Save changes"  </t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO tentar alterar a senha nova para uma igual à atual</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO deixo campos obrigatórios (ex: "First name") em branco  
+E clico no botão "Save changes"  </t>
   </si>
   <si>
-    <t>ENTÃO deve exibir a mensagem "New password cannot be the same as the current password."</t>
+    <t>ENTÃO deve ser exibida a mensagem "First name is a required field."</t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO tentar salvar informações com campos contendo caracteres especiais ou código malicioso</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO tento alterar a senha informando uma senha atual incorreta  </t>
   </si>
   <si>
-    <t>ENTÃO o sistema deve impedir o envio
+    <t>ENTÃO deve ser exibida a mensagem "Current password is incorrect."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO tento alterar a senha nova para uma igual à senha atual  </t>
+  </si>
+  <si>
+    <t>ENTÃO deve ser exibida a mensagem "New password cannot be the same as the current password."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO tento salvar informações com campos contendo caracteres especiais ou código malicioso  </t>
+  </si>
+  <si>
+    <t>ENTÃO o sistema deve impedir o envio  
 E exibir uma mensagem de erro genérica (proteção contra XSS)</t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO a sessão expirar após um tempo de inatividade</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO a sessão expira após um período de inatividade  </t>
   </si>
   <si>
-    <t>ENTÃO deve redirecionar automaticamente para a tela de login
+    <t>ENTÃO deve redirecionar automaticamente para a tela de login  
 E exibir a mensagem "Your session has expired. Please log in again."</t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO houver falha temporária no servidor ao salvar alterações do perfil</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO ocorre uma falha temporária no servidor ao salvar alterações do perfil  </t>
   </si>
   <si>
-    <t>ENTÃO deve exibir a mensagem "An error occurred while saving your changes. Please try again later."</t>
+    <t>ENTÃO deve ser exibida a mensagem "An error occurred while saving your changes. Please try again later."</t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO perder a conexão com a internet durante a atualização dos dados</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO perco a conexão com a internet durante a atualização dos dados  </t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO tentar acessar uma seção restrita sem permissão</t>
+    <t>ENTÃO deve ser exibida a mensagem "Connection error. Please check your internet and try again."</t>
   </si>
   <si>
-    <t>ENTÃO deve exibir a mensagem "You do not have permission to access this section."</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO tento acessar uma seção restrita sem permissão  </t>
   </si>
   <si>
-    <t>DADO que estou logada na área "My Account"
-QUANDO ocorrer falha de sincronização entre o cliente e o servidor</t>
+    <t>ENTÃO deve ser exibida a mensagem "You do not have permission to access this section."</t>
   </si>
   <si>
-    <t>ENTÃO o sistema deve exibir uma mensagem "Your data could not be updated. Please refresh and try again."</t>
+    <t xml:space="preserve">DADO que estou autenticada na área "My Account"  
+QUANDO ocorre falha de sincronização entre o cliente e o servidor  </t>
   </si>
   <si>
-    <t>ENTÃO deve exibir a lista de pedidos caso o usuário tenha</t>
-  </si>
-  <si>
-    <t>ENTÃO deve exibir a lista de produtos disponíveis para download caso usuário tenha</t>
-  </si>
-  <si>
-    <t>ENTÃO deve exibir os endereços de cobrança e entrega caso usuário tenha cadastrado</t>
-  </si>
-  <si>
-    <t>ENTÃO deve exibir os campos "First name", "Last name", "Password change" E o botão "SAVE CHANGES"</t>
-  </si>
-  <si>
-    <t>ENTÃO deve salvar as alterações 
-E deve exibir a mensagem: "Account details changed successfully."</t>
+    <t>ENTÃO deve ser exibida a mensagem "Your data could not be updated. Please refresh and try again."</t>
   </si>
 </sst>
 </file>
@@ -662,7 +663,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -691,12 +692,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -781,7 +776,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -876,9 +871,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -38829,7 +38821,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -38872,7 +38864,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
@@ -38965,7 +38957,7 @@
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="16"/>
@@ -38981,7 +38973,7 @@
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="16"/>
@@ -38997,7 +38989,7 @@
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="16"/>
@@ -39013,7 +39005,7 @@
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="16"/>
@@ -39059,7 +39051,7 @@
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="16"/>
@@ -39075,7 +39067,7 @@
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="16"/>
@@ -39086,12 +39078,12 @@
         <v>10</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="16"/>
@@ -39102,12 +39094,12 @@
         <v>11</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="16"/>
@@ -43065,7 +43057,7 @@
   <dimension ref="A1:W994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:C17"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -43110,7 +43102,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -43148,7 +43140,7 @@
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
       <c r="I5" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
@@ -43221,7 +43213,7 @@
       <c r="V9" s="18"/>
       <c r="W9" s="18"/>
     </row>
-    <row r="10" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>1</v>
       </c>
@@ -43239,7 +43231,6 @@
     </row>
     <row r="11" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
-        <f t="shared" ref="A11:A27" si="0">A10+1</f>
         <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -43256,7 +43247,6 @@
     </row>
     <row r="12" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -43265,7 +43255,7 @@
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="19" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="16"/>
@@ -43273,16 +43263,15 @@
     </row>
     <row r="13" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="16">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="19" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="16"/>
@@ -43290,16 +43279,15 @@
     </row>
     <row r="14" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="16">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="19" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="16"/>
@@ -43307,67 +43295,63 @@
     </row>
     <row r="15" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="16">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="19" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="16"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A16" s="16">
-        <f>A17+1</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="19" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="16"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="35">
-        <f>A15+1</f>
-        <v>7</v>
+    <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="16">
+        <v>8</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="19" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="16"/>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A18" s="16">
-        <f>A16+1</f>
         <v>9</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="19" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="16"/>
@@ -43375,16 +43359,15 @@
     </row>
     <row r="19" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A19" s="16">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="19" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="16"/>
@@ -43392,16 +43375,15 @@
     </row>
     <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="16">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="19" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="16"/>
@@ -43409,16 +43391,15 @@
     </row>
     <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="16">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="19" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="16"/>
@@ -43426,16 +43407,15 @@
     </row>
     <row r="22" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A22" s="16">
-        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="19" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="16"/>
@@ -43443,16 +43423,15 @@
     </row>
     <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="16">
-        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="19" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="16"/>
@@ -43460,16 +43439,15 @@
     </row>
     <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="16">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="19" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="16"/>
@@ -43477,16 +43455,15 @@
     </row>
     <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="16">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="19" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="16"/>
@@ -43494,16 +43471,15 @@
     </row>
     <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="16">
-        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="19" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="16"/>
@@ -43511,16 +43487,15 @@
     </row>
     <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="16">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="19" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="16"/>
@@ -47432,19 +47407,19 @@
           <x14:formula1>
             <xm:f>macros!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D18:D27 D10:D17</xm:sqref>
+          <xm:sqref>D10:D27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{984DFAA4-DA1B-4273-8667-742082635EED}">
           <x14:formula1>
             <xm:f>macros!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C18:C27 C10:C17</xm:sqref>
+          <xm:sqref>C10:C27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{FFFE94E2-B9BE-4313-B5E9-E9501D0F00C7}">
           <x14:formula1>
             <xm:f>macros!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H18:H27 H10:H17</xm:sqref>
+          <xm:sqref>H10:H27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>